<commit_message>
Moving to correct folder
Moving RACI Matrix from outside folder into folder and then deleting the out-of-folder one
</commit_message>
<xml_diff>
--- a/RACI-Matrix/RACI Matrix.xlsx
+++ b/RACI-Matrix/RACI Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sheffieldhallam-my.sharepoint.com/personal/c3028707_hallam_shu_ac_uk/Documents/Final year/Managment of I.T/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="504" documentId="8_{41C1BABE-DF25-4410-9D73-72180097358A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E2FAD7F-49CA-4948-AF25-891BBF61CB19}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{7E61B2B3-DABE-4EF1-805E-1270D82B2E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96FAA38E-AA69-42F6-9671-A5AEC3AE26A4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D7E09A9A-AB23-4A5F-B8A2-08E6275B13B1}"/>
+    <workbookView xWindow="30825" yWindow="2310" windowWidth="21810" windowHeight="15345" xr2:uid="{D7E09A9A-AB23-4A5F-B8A2-08E6275B13B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="56">
   <si>
     <t>RACI Matrix</t>
   </si>
@@ -96,63 +96,6 @@
   </si>
   <si>
     <t>Packages/Tasks</t>
-  </si>
-  <si>
-    <t>Planning</t>
-  </si>
-  <si>
-    <t>Cost Management</t>
-  </si>
-  <si>
-    <t>Task Management</t>
-  </si>
-  <si>
-    <t>Risk Management</t>
-  </si>
-  <si>
-    <t>Quality Management</t>
-  </si>
-  <si>
-    <t>wireframe</t>
-  </si>
-  <si>
-    <t>Branding Integration</t>
-  </si>
-  <si>
-    <t>High fidelity Prototype</t>
-  </si>
-  <si>
-    <t>Map API provider</t>
-  </si>
-  <si>
-    <t>Cloud Hosting</t>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
-    <t>Force Field Analysis</t>
-  </si>
-  <si>
-    <t>COCOMO II</t>
-  </si>
-  <si>
-    <t>GANTT Chart</t>
-  </si>
-  <si>
-    <t>Compile runbooks</t>
-  </si>
-  <si>
-    <t>Confirm access information</t>
-  </si>
-  <si>
-    <t>Define support window</t>
-  </si>
-  <si>
-    <t>final sign-off</t>
-  </si>
-  <si>
-    <t>Video walkthrough</t>
   </si>
   <si>
     <t>people who does the work</t>
@@ -169,12 +112,6 @@
 progress and decisions</t>
   </si>
   <si>
-    <t>Business Case</t>
-  </si>
-  <si>
-    <t>Use Case Diagrams</t>
-  </si>
-  <si>
     <t>Steering Group</t>
   </si>
   <si>
@@ -187,16 +124,88 @@
     <t xml:space="preserve">Business Analyst </t>
   </si>
   <si>
-    <t>Final Deployed Software</t>
-  </si>
-  <si>
-    <t>Source Code</t>
-  </si>
-  <si>
-    <t>Test Report</t>
-  </si>
-  <si>
-    <t>Deployment Document</t>
+    <t>1.1.1 Planning</t>
+  </si>
+  <si>
+    <t>1.1.1.1 Business Case</t>
+  </si>
+  <si>
+    <t>1.1.1.2 Force Field Analysis</t>
+  </si>
+  <si>
+    <t>1.1.1.3 COCOMO II</t>
+  </si>
+  <si>
+    <t>1.1.2 Risk Management</t>
+  </si>
+  <si>
+    <t>1.1.3 Task Management</t>
+  </si>
+  <si>
+    <t>1.1.1.4 Cost Management</t>
+  </si>
+  <si>
+    <t>1.1.4 RACI Matrix</t>
+  </si>
+  <si>
+    <t>1.1.1.5 GANTT Chart</t>
+  </si>
+  <si>
+    <t>1.1.1.6 Use Case Diagrams</t>
+  </si>
+  <si>
+    <t>1.1.5 Quality Management</t>
+  </si>
+  <si>
+    <t>1.2.1 wireframe</t>
+  </si>
+  <si>
+    <t>1.2.2 Branding Integration</t>
+  </si>
+  <si>
+    <t>1.2.3 High fidelity Prototype</t>
+  </si>
+  <si>
+    <t>1.2.4 Video walkthrough</t>
+  </si>
+  <si>
+    <t>1.3.1 Map API provider</t>
+  </si>
+  <si>
+    <t>1.4.1 Final Deployed Software</t>
+  </si>
+  <si>
+    <t>1.4.3 Test Report</t>
+  </si>
+  <si>
+    <t>1.4.4 Deployment Document</t>
+  </si>
+  <si>
+    <t>1.5.1 Compile runbooks</t>
+  </si>
+  <si>
+    <t>1.5.2 Confirm access information</t>
+  </si>
+  <si>
+    <t>1.5.2 Define support window</t>
+  </si>
+  <si>
+    <t>1.5.4 final sign-off</t>
+  </si>
+  <si>
+    <t>1.3.2 Cloud Hosting</t>
+  </si>
+  <si>
+    <t>1.3.3 Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.1.7 work breakdown structure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.1.8 MoSCoW  analysis </t>
+  </si>
+  <si>
+    <t>1.4.2 Source Code</t>
   </si>
 </sst>
 </file>
@@ -407,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -462,6 +471,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,10 +539,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -850,21 +858,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DBE0A5-4976-4982-AD55-590A37ED2436}">
-  <dimension ref="B5:N44"/>
+  <dimension ref="B5:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="81" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="81" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" customWidth="1"/>
-    <col min="5" max="14" width="6.88671875" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="5" max="14" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:14" ht="63" x14ac:dyDescent="1.2">
+    <row r="5" spans="2:14" ht="63.75" x14ac:dyDescent="1">
       <c r="F5" s="20" t="s">
         <v>0</v>
       </c>
@@ -875,7 +883,7 @@
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
     </row>
-    <row r="7" spans="2:14" ht="18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>1</v>
       </c>
@@ -883,10 +891,10 @@
         <v>5</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" ht="18" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>2</v>
       </c>
@@ -894,10 +902,10 @@
         <v>6</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>3</v>
       </c>
@@ -905,10 +913,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
         <v>4</v>
       </c>
@@ -916,10 +924,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -931,7 +939,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -943,7 +951,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -955,7 +963,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="2:14" ht="133.80000000000001" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" ht="139.5" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
@@ -972,7 +980,7 @@
         <v>12</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>17</v>
@@ -990,30 +998,30 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="19"/>
       <c r="H16" s="17" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="I16" s="18"/>
       <c r="J16" s="19"/>
       <c r="K16" s="17" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="L16" s="18"/>
       <c r="M16" s="18"/>
       <c r="N16" s="19"/>
     </row>
-    <row r="17" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>1</v>
@@ -1044,9 +1052,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D18" s="5" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>1</v>
@@ -1079,12 +1087,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D19" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>4</v>
@@ -1106,9 +1114,9 @@
       </c>
       <c r="N19" s="6"/>
     </row>
-    <row r="20" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>3</v>
@@ -1130,18 +1138,18 @@
         <v>4</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N20" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D21" s="5" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>1</v>
@@ -1170,52 +1178,57 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D22" s="5" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H22" s="6"/>
       <c r="I22" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J22" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="K22" s="6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L22" s="6" t="s">
         <v>3</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D23" s="5" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H23" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="I23" s="6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>4</v>
@@ -1224,184 +1237,183 @@
         <v>4</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M23" s="6" t="s">
         <v>4</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" s="5" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="L24" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N24" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D25" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L25" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N25" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N26" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D27" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="E27" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H27" s="6"/>
       <c r="I27" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K27" s="6"/>
+      <c r="K27" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="L27" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D28" s="5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M28" s="6" t="s">
         <v>4</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D29" s="5" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>4</v>
@@ -1409,25 +1421,29 @@
       <c r="G29" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H29" s="6"/>
+      <c r="H29" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="I29" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K29" s="6"/>
       <c r="L29" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M29" s="6"/>
+      <c r="M29" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="N29" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D30" s="5" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>4</v>
@@ -1442,16 +1458,14 @@
         <v>3</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K30" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="K30" s="6"/>
       <c r="L30" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M30" s="6" t="s">
         <v>4</v>
@@ -1460,12 +1474,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D31" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>4</v>
@@ -1475,30 +1489,26 @@
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K31" s="6"/>
       <c r="L31" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="M31" s="6"/>
       <c r="N31" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D32" s="5" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>4</v>
@@ -1506,28 +1516,34 @@
       <c r="G32" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H32" s="6"/>
+      <c r="H32" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I32" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J32" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="K32" s="6" t="s">
         <v>4</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N32" s="6"/>
-    </row>
-    <row r="33" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D33" s="5" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>4</v>
@@ -1539,26 +1555,28 @@
       <c r="I33" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J33" s="6"/>
+      <c r="J33" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="K33" s="6" t="s">
         <v>4</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N33" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D34" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>4</v>
@@ -1568,7 +1586,7 @@
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6" t="s">
@@ -1582,12 +1600,12 @@
       </c>
       <c r="N34" s="6"/>
     </row>
-    <row r="35" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D35" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>4</v>
@@ -1595,20 +1613,16 @@
       <c r="G35" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="H35" s="6"/>
       <c r="I35" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="J35" s="6"/>
       <c r="K35" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M35" s="6" t="s">
         <v>1</v>
@@ -1617,24 +1631,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D36" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F36" s="6"/>
+      <c r="F36" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="G36" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="J36" s="6"/>
       <c r="K36" s="6" t="s">
         <v>4</v>
       </c>
@@ -1644,16 +1658,14 @@
       <c r="M36" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="N36" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N36" s="6"/>
+    </row>
+    <row r="37" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D37" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>4</v>
@@ -1671,34 +1683,30 @@
         <v>4</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M37" s="6" t="s">
         <v>1</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D38" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F38" s="6"/>
       <c r="G38" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H38" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="H38" s="6"/>
       <c r="I38" s="6" t="s">
         <v>4</v>
       </c>
@@ -1706,10 +1714,10 @@
         <v>4</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M38" s="6" t="s">
         <v>1</v>
@@ -1718,9 +1726,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D39" s="5" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>3</v>
@@ -1731,30 +1739,34 @@
       <c r="G39" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H39" s="6"/>
+      <c r="H39" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I39" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J39" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="K39" s="6" t="s">
         <v>4</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M39" s="6" t="s">
         <v>1</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D40" s="5" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>4</v>
@@ -1762,29 +1774,37 @@
       <c r="G40" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
+      <c r="H40" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="J40" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K40" s="6"/>
+      <c r="K40" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="L40" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M40" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="N40" s="6"/>
-    </row>
-    <row r="41" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N40" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D41" s="5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>4</v>
@@ -1794,52 +1814,110 @@
         <v>4</v>
       </c>
       <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
+      <c r="K41" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="L41" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N41" s="6"/>
-    </row>
-    <row r="42" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="N41" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D42" s="5" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I42" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
       <c r="J42" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="K42" s="6"/>
       <c r="L42" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N42" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>1</v>
+      </c>
+      <c r="N42" s="6"/>
+    </row>
+    <row r="43" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N43" s="6"/>
+    </row>
+    <row r="44" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N44" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="4:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E16:G16"/>
@@ -1848,7 +1926,7 @@
     <mergeCell ref="F5:L5"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17:N42" xr:uid="{848F6308-B896-4B3C-BA3E-08CFFCD8A229}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17:N44" xr:uid="{848F6308-B896-4B3C-BA3E-08CFFCD8A229}">
       <formula1>$B$7:$B$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -1922,7 +2000,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E17:N42</xm:sqref>
+          <xm:sqref>E17:N44</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>